<commit_message>
Add analog waveform generator
</commit_message>
<xml_diff>
--- a/labview/Subsytem Mapping.xlsx
+++ b/labview/Subsytem Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>UID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -113,7 +113,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>offset</t>
+    <t>increment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of elements</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4..1026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOOL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>active?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>idle offset</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -176,22 +224,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,77 +521,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="24.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" style="5" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
@@ -576,7 +624,7 @@
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -590,7 +638,7 @@
       <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -604,7 +652,7 @@
       <c r="J5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -639,12 +687,69 @@
       <c r="J7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="H9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="H11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="B1:B2"/>
@@ -652,7 +757,6 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add waveform generator update rate
</commit_message>
<xml_diff>
--- a/labview/Subsytem Mapping.xlsx
+++ b/labview/Subsytem Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>UID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,10 +57,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Analog Output</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Register</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,10 +129,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4..1026</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BOOL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -162,6 +154,30 @@
   </si>
   <si>
     <t>idle offset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5..1026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AO0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AO1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -236,10 +252,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,59 +552,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7" t="s">
-        <v>18</v>
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="K2" s="6"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -619,13 +635,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -633,13 +649,13 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -647,18 +663,18 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1">
         <v>32769</v>
@@ -682,13 +698,13 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -696,13 +712,13 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -710,13 +726,13 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -727,24 +743,143 @@
         <v>25</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="H11" s="1">
+        <v>4</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="H12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1">
+        <v>32770</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="H11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="J15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="1" t="s">
+    </row>
+    <row r="16" spans="1:14">
+      <c r="H16" s="1">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11">
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11">
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11">
+      <c r="H19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>